<commit_message>
ADD automatic turno with date
</commit_message>
<xml_diff>
--- a/react-website-bodega/boletas/Boletas profesores.xlsx
+++ b/react-website-bodega/boletas/Boletas profesores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeyki\Desktop\bodega-tec\BODEGA_FRONTEND\react-website-bodega\boletas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A3E403-4ACE-4AC4-8CE0-A5A5FF80F268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AE6A14-6A84-4C8F-A03D-F62458FBB69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{59892FC8-4C31-4DF4-BC32-FCE3D8BCDEAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>BOLETA DE SOLICITUD DE EQUIPO PARA PROFESORES</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Observaciones:</t>
   </si>
   <si>
-    <t>Escuela:</t>
-  </si>
-  <si>
     <t>#Activo</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>Fecha:</t>
+  </si>
+  <si>
+    <t>Carné:</t>
+  </si>
+  <si>
+    <t>Aprobado por:</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -214,11 +217,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -238,41 +278,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71264D3E-8E51-4874-BF66-AD90AF53631E}">
-  <dimension ref="B7:I26"/>
+  <dimension ref="B7:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:H26"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="75" zoomScaleNormal="70" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,43 +708,43 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:9" s="1" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="2:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="2:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -780,112 +829,124 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:8" s="1" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="1" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="2:8" s="1" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" s="1" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="2:8" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="2:8" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="2:8" s="1" customFormat="1" ht="42.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="14"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="2:8" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="2:8" s="1" customFormat="1" ht="42.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="17"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B21:F26"/>
-    <mergeCell ref="G21:H26"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
+  <mergeCells count="18">
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="B22:F27"/>
+    <mergeCell ref="G22:H27"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>